<commit_message>
#3 update control panel lastest
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>nguyen</t>
+          <t>Nguyên</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-01-09 18:50:21</t>
+          <t>2025-01-11 12:33:22</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">

</xml_diff>